<commit_message>
Dummy Commit to Pull Files
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/loginTest_Positive.xlsx
+++ b/src/test/resources/Excel Files/loginTest_Positive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Deepak Patil</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>Ajish V K</t>
+  </si>
+  <si>
+    <t>Ajish</t>
   </si>
 </sst>
 </file>
@@ -70,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -93,6 +102,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -101,10 +121,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -400,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -446,6 +467,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>